<commit_message>
Replaced RTC circuitry/changed bus buffers to available components
</commit_message>
<xml_diff>
--- a/PCB_SDRAM/Default Configuration/Outputs/BOM/BOM_PartType-InterfaceSDRAM.xlsx
+++ b/PCB_SDRAM/Default Configuration/Outputs/BOM/BOM_PartType-InterfaceSDRAM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C45003A-CCFB-4426-AE12-3B1DEB5E3AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99637415-638D-4DAF-A578-8A2F527B54C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30210" yWindow="2385" windowWidth="19530" windowHeight="6000" xr2:uid="{F58B9C77-93FE-4392-BBB6-9FDFBA0DCE87}"/>
+    <workbookView xWindow="30210" yWindow="2385" windowWidth="19530" windowHeight="6000" xr2:uid="{DB994FA0-74C6-4E3C-A773-F66A6C187873}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-InterfaceSDRAM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="102">
   <si>
     <t>Comment</t>
   </si>
@@ -49,6 +49,24 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Battery Holder (Open) Coin, 12.0mm 1 Cell SMD (SMT) Tab</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>BC501SM-TR-ND</t>
+  </si>
+  <si>
+    <t>MPD</t>
+  </si>
+  <si>
+    <t>BC501SM-TR</t>
+  </si>
+  <si>
     <t>0.1UF</t>
   </si>
   <si>
@@ -160,7 +178,7 @@
     <t>RES 4.99K OHM 1/10W 1% 0603 SMD</t>
   </si>
   <si>
-    <t>R7, R9, R10, R11, R125, R126, R127, R128, R129, R130, R131, R132, R133</t>
+    <t>R7, R9, R10, R11, R125, R126, R127, R128, R129, R130, R131, R132, R133, R136, R137</t>
   </si>
   <si>
     <t>541-3985-1-ND</t>
@@ -244,28 +262,34 @@
     <t>1568-1235-ND</t>
   </si>
   <si>
-    <t>RTC3013</t>
-  </si>
-  <si>
-    <t>DS3231 Real Time Clock (RTC) Timing Evaluation Board</t>
+    <t>DS3231SN#</t>
+  </si>
+  <si>
+    <t>Real Time Clock (RTC) IC Clock/Calendar I²C, 2-Wire Serial 16-SOIC (0.295", 7.50mm Width)</t>
   </si>
   <si>
     <t>U5</t>
   </si>
   <si>
-    <t>1528-1598-ND</t>
-  </si>
-  <si>
-    <t>AdaFruit</t>
-  </si>
-  <si>
-    <t>3013</t>
-  </si>
-  <si>
-    <t>74LVX3245</t>
+    <t>DS3231SN#-ND</t>
+  </si>
+  <si>
+    <t>Maxim</t>
+  </si>
+  <si>
+    <t>SN74LVC8T245DWR</t>
+  </si>
+  <si>
+    <t>Voltage Level Translator Bidirectional 1 Circuit 8 Channel 24-SOIC</t>
   </si>
   <si>
     <t>U6, U7, U8, U9</t>
+  </si>
+  <si>
+    <t>296-23280-1-ND</t>
+  </si>
+  <si>
+    <t>TI</t>
   </si>
   <si>
     <t>74LHCT125D</t>
@@ -690,8 +714,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D47B97-2D49-42CB-ADB5-6C8B19363E87}">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B7EFD1-BC9A-463A-BDD9-574739089E4C}">
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -737,59 +761,59 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,7 +836,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -849,13 +873,13 @@
         <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -863,22 +887,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -886,71 +910,71 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G10" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="G11" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,7 +997,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="3">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -981,42 +1005,42 @@
         <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="G13" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1059,10 +1083,10 @@
         <v>71</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
@@ -1070,22 +1094,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -1096,90 +1120,113 @@
         <v>78</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="G18" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="G19" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="G21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>